<commit_message>
Code and tool Excel completition
</commit_message>
<xml_diff>
--- a/CheckLists/Lab01_ReviewReport.xlsx
+++ b/CheckLists/Lab01_ReviewReport.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\facultate\an3-sem2\VVSS\PizzaShop\CheckLists\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FD1D53-39C8-47F8-B5D6-292E3F11D6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" tabRatio="650" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -12,12 +18,25 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -115,20 +134,145 @@
     <t>Tool-based Code Analysis</t>
   </si>
   <si>
-    <t>Effort to perform tool-based code analysis (hours):</t>
+    <t>KitchenGUIController.java:52</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>There is not a verification to dermine if the List is empty or not</t>
+  </si>
+  <si>
+    <t>There is not a handle to manage the apparition of a NullPointerException</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>Main.Java:51, KitchenGUI:37, …</t>
+  </si>
+  <si>
+    <t>There are multiple appearances of unneeded decision functions</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>KitchenGUIController.java:60, KitchenGUIController.java:52</t>
+  </si>
+  <si>
+    <t>There is a violation when calling "toString" for a null element</t>
+  </si>
+  <si>
+    <t>22.3.202024</t>
+  </si>
+  <si>
+    <t>V.D.R. Security</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>KitchenGUIController.java:28</t>
+  </si>
+  <si>
+    <t>There is an undefined loop termination, that loop will end only when killing the program</t>
+  </si>
+  <si>
+    <t>MainGUIController.java:56</t>
+  </si>
+  <si>
+    <t>Empty method is a bad practice and can lead to confusion</t>
+  </si>
+  <si>
+    <t>Added a comment explaining why the method is empty</t>
+  </si>
+  <si>
+    <t>MenuRepository.java:23</t>
+  </si>
+  <si>
+    <t>Streams need to be closed after use</t>
+  </si>
+  <si>
+    <t>try {
+            br = new BufferedReader(new FileReader(file));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      try (BufferedReader br = new BufferedReader(new FileReader(file))) ,             Changed try to try-with-resources</t>
+  </si>
+  <si>
+    <t>Loop needs to have an end condition</t>
+  </si>
+  <si>
+    <t>while (true) {</t>
+  </si>
+  <si>
+    <t>A button that determines the closing of the restaturant needs to be added</t>
+  </si>
+  <si>
+    <t>public MainGUIController(){}</t>
+  </si>
+  <si>
+    <t>PaymentAlert.java:18</t>
+  </si>
+  <si>
+    <t>Define a constant instead of duplicationg  the string</t>
+  </si>
+  <si>
+    <t>System.out.println("--------------------------");</t>
+  </si>
+  <si>
+    <t>System.out.println(paymentAlertDelimitator);</t>
+  </si>
+  <si>
+    <t>PayementType.java:4</t>
+  </si>
+  <si>
+    <t>Constant name has to mach regular expresion ^[A-Z][A-Z0-9]*(_[A-Z0-9]+)*$</t>
+  </si>
+  <si>
+    <t>Cash, Card</t>
+  </si>
+  <si>
+    <t>CASH, CARD</t>
+  </si>
+  <si>
+    <t>Effort to perform tool-based code analysis (hours): 2</t>
+  </si>
+  <si>
+    <t>22.3.2024</t>
+  </si>
+  <si>
+    <t>Unguroiu Victor</t>
+  </si>
+  <si>
+    <t>Patru Denis-Marian</t>
+  </si>
+  <si>
+    <t>Petrutiu Rares-Dan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -300,78 +444,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -383,14 +540,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -428,7 +588,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -500,7 +660,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -673,105 +833,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.41796875" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.89453125" style="6"/>
+    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="14" t="s">
+      <c r="I3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="20">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="24"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="14" t="s">
+      <c r="I4" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="37">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="26"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="37">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -781,11 +953,11 @@
       <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -793,7 +965,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -802,7 +974,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -811,7 +983,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -820,7 +992,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -829,7 +1001,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -838,7 +1010,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -847,7 +1019,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -856,86 +1028,83 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="12" t="s">
+      <c r="E25" s="15"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="13"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="1"/>
     </row>
   </sheetData>
@@ -953,104 +1122,116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="22.05078125" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="22" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="20">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="27"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="37">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="29"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="37">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1064,7 +1245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1072,7 +1253,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1081,7 +1262,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1090,7 +1271,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1099,7 +1280,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1108,7 +1289,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1117,7 +1298,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1126,7 +1307,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1135,7 +1316,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1144,7 +1325,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1153,7 +1334,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1162,7 +1343,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1171,7 +1352,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1180,7 +1361,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1189,7 +1370,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1198,7 +1379,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1207,7 +1388,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1216,14 +1397,11 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="12" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="13"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="1"/>
     </row>
   </sheetData>
@@ -1241,105 +1419,121 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="26.734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="17" t="s">
+      <c r="I3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="20">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="30"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="17" t="s">
+      <c r="I4" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="37">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="32"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="37">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1353,51 +1547,81 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1406,7 +1630,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1415,7 +1639,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1424,7 +1648,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1433,7 +1657,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1442,7 +1666,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1451,7 +1675,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1460,7 +1684,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1469,7 +1693,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1478,7 +1702,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1487,7 +1711,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1496,7 +1720,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1505,7 +1729,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1514,7 +1738,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1523,7 +1747,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1532,7 +1756,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1541,15 +1765,14 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="12" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="1"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1566,96 +1789,113 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.9453125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.62890625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="26.734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="6" customWidth="1"/>
+    <col min="6" max="7" width="38.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="38" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="38"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="17" t="s">
+      <c r="I3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="20">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="H4" s="18" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="37">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="H5" s="18" t="s">
+      <c r="D5" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="37">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1672,56 +1912,96 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1731,7 +2011,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1741,7 +2021,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1751,7 +2031,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1761,7 +2041,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1771,7 +2051,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1781,7 +2061,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1791,7 +2071,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1801,7 +2081,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1811,7 +2091,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1821,7 +2101,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1831,7 +2111,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1841,7 +2121,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1851,7 +2131,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1861,7 +2141,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1871,7 +2151,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1881,16 +2161,13 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="19"/>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>